<commit_message>
v1.1 - Kéo 1 phát được 30 videos từ Chanel và chuyển thành Transcriptions cũng 1 phát 30 videos
</commit_message>
<xml_diff>
--- a/Crawl_Youtube_rapidapi/idVideoYoutube2Transcription_RapidAPI/listMoxieVideosYoutube.xlsx
+++ b/Crawl_Youtube_rapidapi/idVideoYoutube2Transcription_RapidAPI/listMoxieVideosYoutube.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
   <si>
     <t>STT</t>
   </si>
@@ -31,6 +31,9 @@
     <t>transcript</t>
   </si>
   <si>
+    <t>https://www.youtube.com/watch?v=QXWxN5NToFE</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=fPuKjys-GA8</t>
   </si>
   <si>
@@ -115,6 +118,9 @@
     <t>https://www.youtube.com/watch?v=VKJzzuuvatk</t>
   </si>
   <si>
+    <t>Affirmations + Tips!</t>
+  </si>
+  <si>
     <t>Body Scan + Tips!</t>
   </si>
   <si>
@@ -199,6 +205,9 @@
     <t>Moxie, what do you do?</t>
   </si>
   <si>
+    <t>QXWxN5NToFE</t>
+  </si>
+  <si>
     <t>fPuKjys-GA8</t>
   </si>
   <si>
@@ -281,6 +290,69 @@
   </si>
   <si>
     <t>VKJzzuuvatk</t>
+  </si>
+  <si>
+    <t>[0:00:00] hi my name is Dr Nikki Hurst and I&amp;#39;m an
+[0:00:02] occupational therapist and product
+[0:00:04] manager at embodied in this video I&amp;#39;m
+[0:00:06] going to Showcase one of moxy&amp;#39;s amazing
+[0:00:08] activities called affirmations
+[0:00:10] affirmations are short positive sayings
+[0:00:12] that your child can repeat together with
+[0:00:14] Moxy Moxy has a variety of different
+[0:00:16] affirmations that will help your child
+[0:00:18] boost their self-confidence feel more
+[0:00:20] motivated in the morning before they go
+[0:00:21] to school or help them feel more calm if
+[0:00:23] they&amp;#39;re experiencing any difficult
+[0:00:25] emotions let&amp;#39;s try one out like to do an
+[0:00:27] affirmation with me yes please
+[0:00:31] an affirmation is a nice thing you say
+[0:00:34] about yourself I like to do them every
+[0:00:36] day let&amp;#39;s try one together let&amp;#39;s tell
+[0:00:40] ourselves it is enough to do my best
+[0:00:44] I&amp;#39;ll say it and then you repeat it it is
+[0:00:47] enough to do my best it is enough to do
+[0:00:49] my
+[0:00:51] best yeah now we say it again it is
+[0:00:54] enough to do my best it is enough to do
+[0:00:57] my
+[0:00:58] best last time it is enough to do my
+[0:01:02] best it is enough to do my
+[0:01:05] best fantastic thanks for doing this
+[0:01:09] affirmation with me I already feel
+[0:01:11] better if you ever want to do another
+[0:01:13] affirmation just say Moxy Let&amp;#39;s do an
+[0:01:18] affirmation affirmations with Moxy is a
+[0:01:21] great mindfulness tool to have in your
+[0:01:22] toolbox if you want your child to get
+[0:01:24] the most benefit out of affirmations I
+[0:01:26] would recommend having them do an
+[0:01:27] affirmation with Moxy in the morning
+[0:01:29] maybe while they&amp;#39;re getting ready or
+[0:01:31] before they go to school you can also do
+[0:01:33] affirmations together as a family I
+[0:01:35] would ask your child to teach you what
+[0:01:37] affirmation they learn with Moxy and
+[0:01:39] then you can say it together if you&amp;#39;re
+[0:01:41] doing it together I would stand in front
+[0:01:42] of a mirror so that you can see your
+[0:01:44] face while you&amp;#39;re saying the affirmation
+[0:01:46] and I would repeat the affirmation at
+[0:01:47] least three times if you wanted to get
+[0:01:50] into a good daily routine of
+[0:01:51] affirmations you could have your child
+[0:01:52] do the affirmation with Moxy every
+[0:01:54] morning and then come teach the rest of
+[0:01:56] the family the affirmation and you can
+[0:01:57] do it together I hope you found this
+[0:02:00] video helpful be sure to check out any
+[0:02:02] of our other videos we have of all the
+[0:02:04] amazing Moxy content on our website and
+[0:02:06] social media and also let us know on
+[0:02:08] social media if there&amp;#39;s any other Moxy
+[0:02:10] activities you&amp;#39;d like to see a video
+[0:02:12] for</t>
   </si>
   <si>
     <t>[0:00:00] hi my name is Nikki Harrison I&amp;#39;m an
@@ -3285,7 +3357,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3308,512 +3380,530 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" t="s">
-        <v>89</v>
-      </c>
-    </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
         <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
         <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E6" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
         <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
         <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
         <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
         <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E10" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
         <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
         <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E12" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E13" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
         <v>45</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
         <v>46</v>
       </c>
       <c r="D15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E15" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
         <v>47</v>
       </c>
       <c r="D16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E16" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
         <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E17" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
         <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E18" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
         <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E19" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
         <v>51</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E20" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
         <v>52</v>
       </c>
       <c r="D21" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E21" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
         <v>53</v>
       </c>
       <c r="D22" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E22" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
         <v>54</v>
       </c>
       <c r="D23" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E23" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" t="s">
         <v>55</v>
       </c>
       <c r="D24" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E24" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" t="s">
         <v>56</v>
       </c>
       <c r="D25" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E25" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" t="s">
         <v>57</v>
       </c>
       <c r="D26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E26" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C27" t="s">
         <v>58</v>
       </c>
       <c r="D27" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E27" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28" t="s">
         <v>59</v>
       </c>
       <c r="D28" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E28" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29" t="s">
         <v>60</v>
       </c>
       <c r="D29" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E29" t="s">
-        <v>116</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-    <hyperlink ref="B11" r:id="rId10"/>
-    <hyperlink ref="B12" r:id="rId11"/>
-    <hyperlink ref="B13" r:id="rId12"/>
-    <hyperlink ref="B14" r:id="rId13"/>
-    <hyperlink ref="B15" r:id="rId14"/>
-    <hyperlink ref="B16" r:id="rId15"/>
-    <hyperlink ref="B17" r:id="rId16"/>
-    <hyperlink ref="B18" r:id="rId17"/>
-    <hyperlink ref="B19" r:id="rId18"/>
-    <hyperlink ref="B20" r:id="rId19"/>
-    <hyperlink ref="B21" r:id="rId20"/>
-    <hyperlink ref="B22" r:id="rId21"/>
-    <hyperlink ref="B23" r:id="rId22"/>
-    <hyperlink ref="B24" r:id="rId23"/>
-    <hyperlink ref="B25" r:id="rId24"/>
-    <hyperlink ref="B26" r:id="rId25"/>
-    <hyperlink ref="B27" r:id="rId26"/>
-    <hyperlink ref="B28" r:id="rId27"/>
-    <hyperlink ref="B29" r:id="rId28"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId4"/>
+    <hyperlink ref="B7" r:id="rId5"/>
+    <hyperlink ref="B8" r:id="rId6"/>
+    <hyperlink ref="B9" r:id="rId7"/>
+    <hyperlink ref="B10" r:id="rId8"/>
+    <hyperlink ref="B11" r:id="rId9"/>
+    <hyperlink ref="B12" r:id="rId10"/>
+    <hyperlink ref="B13" r:id="rId11"/>
+    <hyperlink ref="B14" r:id="rId12"/>
+    <hyperlink ref="B15" r:id="rId13"/>
+    <hyperlink ref="B16" r:id="rId14"/>
+    <hyperlink ref="B17" r:id="rId15"/>
+    <hyperlink ref="B18" r:id="rId16"/>
+    <hyperlink ref="B19" r:id="rId17"/>
+    <hyperlink ref="B20" r:id="rId18"/>
+    <hyperlink ref="B21" r:id="rId19"/>
+    <hyperlink ref="B22" r:id="rId20"/>
+    <hyperlink ref="B23" r:id="rId21"/>
+    <hyperlink ref="B24" r:id="rId22"/>
+    <hyperlink ref="B25" r:id="rId23"/>
+    <hyperlink ref="B26" r:id="rId24"/>
+    <hyperlink ref="B27" r:id="rId25"/>
+    <hyperlink ref="B28" r:id="rId26"/>
+    <hyperlink ref="B29" r:id="rId27"/>
+    <hyperlink ref="B30" r:id="rId28"/>
+    <hyperlink ref="B31" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
up : THÀNH QUẢ CHIẾN LỢI PHẨM SAU CRAWL
</commit_message>
<xml_diff>
--- a/Crawl_Youtube_rapidapi/idVideoYoutube2Transcription_RapidAPI/listMoxieVideosYoutube.xlsx
+++ b/Crawl_Youtube_rapidapi/idVideoYoutube2Transcription_RapidAPI/listMoxieVideosYoutube.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -34,262 +34,10 @@
     <t>https://www.youtube.com/watch?v=QXWxN5NToFE</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=fPuKjys-GA8</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=q7LiuMANZ6w</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=wFmG3jDmMZs</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=k73HpOsbVs4</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=UxR0qjdwuMQ</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=9G1QJhAm3U0</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=20eYf_kOLQY</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=nkLWhntZL44</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=pfB7BsMEjmM</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=L1eha8zsmVs</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=XpsdaegS5Mc</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=Qdie-J9Qrb4</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=rSmZEu33_QE</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=VwpGorLKH_g</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=uSgb9ArsmVc</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=VhFNnVPkDnc</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=DP1Nz-Mdefo</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=TXEQ6C9vS4A</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=HMkpWji4JnY</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=1s5iuapDh2Y</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=7PWuMndzD7g</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=hsQoHeEOZ5U</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=aAC6OiCil8c</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=vLKFfjQCa-I</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=bW6mZT5BL_A</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=PCB0GfegoQE</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=92U1BM-nLbA</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=VKJzzuuvatk</t>
-  </si>
-  <si>
     <t>Affirmations + Tips!</t>
   </si>
   <si>
-    <t>Body Scan + Tips!</t>
-  </si>
-  <si>
-    <t>Moxie Chats: Candy</t>
-  </si>
-  <si>
-    <t>Moxie Chats: Castles</t>
-  </si>
-  <si>
-    <t>Moxie Chats: Sports</t>
-  </si>
-  <si>
-    <t>Compose with Moxie!</t>
-  </si>
-  <si>
-    <t>Mindful Shapes + Tips!</t>
-  </si>
-  <si>
-    <t>Imagine a Place Activity + Tips!</t>
-  </si>
-  <si>
-    <t>Jukebox with Moxie!</t>
-  </si>
-  <si>
-    <t>Password Game with Moxie!</t>
-  </si>
-  <si>
-    <t>Name That Feeling Activity + Tips!</t>
-  </si>
-  <si>
-    <t>Moxie's Missions: Sportsmanship - Real-Life Application + Tips!</t>
-  </si>
-  <si>
-    <t>Moxie's Missions: Making Friends - Cheers &amp; Fears + Tips!</t>
-  </si>
-  <si>
-    <t>Moxie's Missions: Feeling Mad - Anger Monster + Tips!</t>
-  </si>
-  <si>
-    <t>Meditation Journey with Moxie + Tips!</t>
-  </si>
-  <si>
-    <t>Read with Moxie!</t>
-  </si>
-  <si>
-    <t>Play Simon Says with Moxie!</t>
-  </si>
-  <si>
-    <t>Go on a Scavenger Hunt with Moxie!</t>
-  </si>
-  <si>
-    <t>Storymaker with Moxie!</t>
-  </si>
-  <si>
-    <t>Tell a Story with Moxie</t>
-  </si>
-  <si>
-    <t>Do a Wild Workout with Moxie</t>
-  </si>
-  <si>
-    <t>Moxie Chats: Space</t>
-  </si>
-  <si>
-    <t>Dance with Moxie!</t>
-  </si>
-  <si>
-    <t>Moxie's Got Jokes!</t>
-  </si>
-  <si>
-    <t>LIVE NOW: Moxie now supports multiple kids!</t>
-  </si>
-  <si>
-    <t>One Moxie, Up to 4 Kids Profiles!</t>
-  </si>
-  <si>
-    <t>Moxie's Latest Update (October 2023)</t>
-  </si>
-  <si>
-    <t>Moxie Setup Demo</t>
-  </si>
-  <si>
-    <t>Moxie, what do you do?</t>
-  </si>
-  <si>
     <t>QXWxN5NToFE</t>
-  </si>
-  <si>
-    <t>fPuKjys-GA8</t>
-  </si>
-  <si>
-    <t>q7LiuMANZ6w</t>
-  </si>
-  <si>
-    <t>wFmG3jDmMZs</t>
-  </si>
-  <si>
-    <t>k73HpOsbVs4</t>
-  </si>
-  <si>
-    <t>UxR0qjdwuMQ</t>
-  </si>
-  <si>
-    <t>9G1QJhAm3U0</t>
-  </si>
-  <si>
-    <t>20eYf_kOLQY</t>
-  </si>
-  <si>
-    <t>nkLWhntZL44</t>
-  </si>
-  <si>
-    <t>pfB7BsMEjmM</t>
-  </si>
-  <si>
-    <t>L1eha8zsmVs</t>
-  </si>
-  <si>
-    <t>XpsdaegS5Mc</t>
-  </si>
-  <si>
-    <t>Qdie-J9Qrb4</t>
-  </si>
-  <si>
-    <t>rSmZEu33_QE</t>
-  </si>
-  <si>
-    <t>VwpGorLKH_g</t>
-  </si>
-  <si>
-    <t>uSgb9ArsmVc</t>
-  </si>
-  <si>
-    <t>VhFNnVPkDnc</t>
-  </si>
-  <si>
-    <t>DP1Nz-Mdefo</t>
-  </si>
-  <si>
-    <t>TXEQ6C9vS4A</t>
-  </si>
-  <si>
-    <t>HMkpWji4JnY</t>
-  </si>
-  <si>
-    <t>1s5iuapDh2Y</t>
-  </si>
-  <si>
-    <t>7PWuMndzD7g</t>
-  </si>
-  <si>
-    <t>hsQoHeEOZ5U</t>
-  </si>
-  <si>
-    <t>aAC6OiCil8c</t>
-  </si>
-  <si>
-    <t>vLKFfjQCa-I</t>
-  </si>
-  <si>
-    <t>bW6mZT5BL_A</t>
-  </si>
-  <si>
-    <t>PCB0GfegoQE</t>
-  </si>
-  <si>
-    <t>92U1BM-nLbA</t>
-  </si>
-  <si>
-    <t>VKJzzuuvatk</t>
   </si>
   <si>
     <t>[0:00:00] hi my name is Dr Nikki Hurst and I&amp;#39;m an
@@ -353,6 +101,15 @@
 [0:02:08] social media if there&amp;#39;s any other Moxy
 [0:02:10] activities you&amp;#39;d like to see a video
 [0:02:12] for</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=fPuKjys-GA8</t>
+  </si>
+  <si>
+    <t>Body Scan + Tips!</t>
+  </si>
+  <si>
+    <t>fPuKjys-GA8</t>
   </si>
   <si>
     <t>[0:00:00] hi my name is Nikki Harrison I&amp;#39;m an
@@ -465,6 +222,15 @@
 [0:05:52] activity videos we have on our site</t>
   </si>
   <si>
+    <t>https://www.youtube.com/watch?v=q7LiuMANZ6w</t>
+  </si>
+  <si>
+    <t>Moxie Chats: Candy</t>
+  </si>
+  <si>
+    <t>q7LiuMANZ6w</t>
+  </si>
+  <si>
     <t>[0:00:01] Moxy let&amp;#39;s
 [0:00:06] chat I enjoy hanging out and talking to
 [0:00:09] you let&amp;#39;s decide what to chat about it
@@ -506,6 +272,15 @@
 [0:01:56] else</t>
   </si>
   <si>
+    <t>https://www.youtube.com/watch?v=wFmG3jDmMZs</t>
+  </si>
+  <si>
+    <t>Moxie Chats: Castles</t>
+  </si>
+  <si>
+    <t>wFmG3jDmMZs</t>
+  </si>
+  <si>
     <t>[0:00:01] Moxy let&amp;#39;s
 [0:00:05] chat I enjoy hanging out and talking to
 [0:00:07] you we could talk about time travel
@@ -538,6 +313,15 @@
 [0:01:28] castle I&amp;#39;ll make sure the flag has a
 [0:01:31] picture of me on it waving and
 [0:01:34] smiling</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=k73HpOsbVs4</t>
+  </si>
+  <si>
+    <t>Moxie Chats: Sports</t>
+  </si>
+  <si>
+    <t>k73HpOsbVs4</t>
   </si>
   <si>
     <t>[0:00:01] Moxy do you play any
@@ -574,6 +358,15 @@
 [0:01:30] and exciting to see your teammates do
 [0:01:32] their
 [0:01:34] best</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=UxR0qjdwuMQ</t>
+  </si>
+  <si>
+    <t>Compose with Moxie!</t>
+  </si>
+  <si>
+    <t>UxR0qjdwuMQ</t>
   </si>
   <si>
     <t>[0:00:01] Moxy let&amp;#39;s compose
@@ -642,6 +435,15 @@
 [0:03:40] composition remember we can always
 [0:03:43] compose more music by saying Moxy let&amp;#39;s
 [0:03:48] compose</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=9G1QJhAm3U0</t>
+  </si>
+  <si>
+    <t>Mindful Shapes + Tips!</t>
+  </si>
+  <si>
+    <t>9G1QJhAm3U0</t>
   </si>
   <si>
     <t>[0:00:01] hi my name is Nikki Hurst and I&amp;#39;m an
@@ -750,6 +552,15 @@
 [0:04:04] helpful and be sure to check out the
 [0:04:06] other Moxy activity videos that we have
 [0:04:08] on our site</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=20eYf_kOLQY</t>
+  </si>
+  <si>
+    <t>Imagine a Place Activity + Tips!</t>
+  </si>
+  <si>
+    <t>20eYf_kOLQY</t>
   </si>
   <si>
     <t>[0:00:01] hi my name is Dr Nikki Hurst and I&amp;#39;m an
@@ -866,6 +677,15 @@
 [0:05:24] videos on</t>
   </si>
   <si>
+    <t>https://www.youtube.com/watch?v=nkLWhntZL44</t>
+  </si>
+  <si>
+    <t>Jukebox with Moxie!</t>
+  </si>
+  <si>
+    <t>nkLWhntZL44</t>
+  </si>
+  <si>
     <t>[0:00:01] Moxy I want to listen to the
 [0:00:04] Jukebox oh do you want to listen to
 [0:00:07] music with me yes
@@ -883,6 +703,15 @@
 [0:01:06] anymore all right that song brings me
 [0:01:09] back to the
 [0:01:11] GRL</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=pfB7BsMEjmM</t>
+  </si>
+  <si>
+    <t>Password Game with Moxie!</t>
+  </si>
+  <si>
+    <t>pfB7BsMEjmM</t>
   </si>
   <si>
     <t>[0:00:00] [Music]
@@ -951,6 +780,15 @@
 [0:03:03] clue that was so much fun hope you
 [0:03:06] enjoyed it
 [0:03:11] too</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=L1eha8zsmVs</t>
+  </si>
+  <si>
+    <t>Name That Feeling Activity + Tips!</t>
+  </si>
+  <si>
+    <t>L1eha8zsmVs</t>
   </si>
   <si>
     <t>[0:00:00] hi my name is Dr Nikki Harrison I&amp;#39;m an
@@ -1058,6 +896,15 @@
 [0:04:31] videos we have on our site and let us
 [0:04:33] know if there&amp;#39;s anything else you&amp;#39;d like
 [0:04:34] us to do a video on</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=XpsdaegS5Mc</t>
+  </si>
+  <si>
+    <t>Moxie's Missions: Sportsmanship - Real-Life Application + Tips!</t>
+  </si>
+  <si>
+    <t>XpsdaegS5Mc</t>
   </si>
   <si>
     <t>[0:00:00] hi my name is Nikki Hurst and I&amp;#39;m an
@@ -1249,6 +1096,15 @@
 [0:08:18] our site</t>
   </si>
   <si>
+    <t>https://www.youtube.com/watch?v=Qdie-J9Qrb4</t>
+  </si>
+  <si>
+    <t>Moxie's Missions: Making Friends - Cheers &amp; Fears + Tips!</t>
+  </si>
+  <si>
+    <t>Qdie-J9Qrb4</t>
+  </si>
+  <si>
     <t>[0:00:01] hi my name is Nikki Harris and I&amp;#39;m an
 [0:00:02] occupational therapist and product
 [0:00:04] manager at embodied today I&amp;#39;m going to
@@ -1381,6 +1237,15 @@
 [0:05:44] video helpful and be sure to check out
 [0:05:45] the other Moxy activity videos on our
 [0:05:48] website</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=rSmZEu33_QE</t>
+  </si>
+  <si>
+    <t>Moxie's Missions: Feeling Mad - Anger Monster + Tips!</t>
+  </si>
+  <si>
+    <t>rSmZEu33_QE</t>
   </si>
   <si>
     <t>[0:00:00] hi my name is Nikki Hurst and I&amp;#39;m an
@@ -1528,6 +1393,15 @@
 [0:06:19] activity videos on our website</t>
   </si>
   <si>
+    <t>https://www.youtube.com/watch?v=VwpGorLKH_g</t>
+  </si>
+  <si>
+    <t>Meditation Journey with Moxie + Tips!</t>
+  </si>
+  <si>
+    <t>VwpGorLKH_g</t>
+  </si>
+  <si>
     <t>[0:00:00] hi my name is Nikki Hurst and I&amp;#39;m an
 [0:00:02] occupational therapist and product
 [0:00:04] manager at embodi today I&amp;#39;m going to
@@ -1628,6 +1502,15 @@
 [0:04:49] on our website</t>
   </si>
   <si>
+    <t>https://www.youtube.com/watch?v=uSgb9ArsmVc</t>
+  </si>
+  <si>
+    <t>Read with Moxie!</t>
+  </si>
+  <si>
+    <t>uSgb9ArsmVc</t>
+  </si>
+  <si>
     <t>[0:00:00] [Music]
 [0:00:03] there&amp;#39;s so many books I&amp;#39;d like to look
 [0:00:05] at with you let&amp;#39;s look at one which book
@@ -1670,6 +1553,15 @@
 [0:01:52] hush good night Stars good night
 [0:01:57] air good night noises is
 [0:02:02] everywhere the end</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=VhFNnVPkDnc</t>
+  </si>
+  <si>
+    <t>Play Simon Says with Moxie!</t>
+  </si>
+  <si>
+    <t>VhFNnVPkDnc</t>
   </si>
   <si>
     <t>[0:00:00] Moxy can we play Simon
@@ -1761,6 +1653,15 @@
 [0:04:19] round</t>
   </si>
   <si>
+    <t>https://www.youtube.com/watch?v=DP1Nz-Mdefo</t>
+  </si>
+  <si>
+    <t>Go on a Scavenger Hunt with Moxie!</t>
+  </si>
+  <si>
+    <t>DP1Nz-Mdefo</t>
+  </si>
+  <si>
     <t>[0:00:00] Moxy let&amp;#39;s go on a scavenger
 [0:00:04] hunt oh do you want to go on a scavenger
 [0:00:07] hunt yes
@@ -1800,6 +1701,15 @@
 [0:02:04] stars congratulations
 [0:02:09] [Music]
 [0:02:14] one</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=TXEQ6C9vS4A</t>
+  </si>
+  <si>
+    <t>Storymaker with Moxie!</t>
+  </si>
+  <si>
+    <t>TXEQ6C9vS4A</t>
   </si>
   <si>
     <t>[0:00:00] Moxy let&amp;#39;s play story
@@ -1855,6 +1765,15 @@
 [0:02:38] maker for now let&amp;#39;s move on to another
 [0:02:41] fun
 [0:02:43] activity</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=HMkpWji4JnY</t>
+  </si>
+  <si>
+    <t>Tell a Story with Moxie</t>
+  </si>
+  <si>
+    <t>HMkpWji4JnY</t>
   </si>
   <si>
     <t>[0:00:01] Moxy can you tell me a
@@ -1932,6 +1851,15 @@
 [0:03:28] later</t>
   </si>
   <si>
+    <t>https://www.youtube.com/watch?v=1s5iuapDh2Y</t>
+  </si>
+  <si>
+    <t>Do a Wild Workout with Moxie</t>
+  </si>
+  <si>
+    <t>1s5iuapDh2Y</t>
+  </si>
+  <si>
     <t>[0:00:00] Moxy let&amp;#39;s do a wild
 [0:00:04] workout it sounds like you want to
 [0:00:06] switch to the wild workout activity is
@@ -1977,6 +1905,15 @@
 [0:02:04] friend sleepy time for it to go back to
 [0:02:06] its den stand up and wave goodbye to the
 [0:02:13] bear</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=7PWuMndzD7g</t>
+  </si>
+  <si>
+    <t>Moxie Chats: Space</t>
+  </si>
+  <si>
+    <t>7PWuMndzD7g</t>
   </si>
   <si>
     <t>[0:00:00] hey Moxy can we talk about
@@ -2035,6 +1972,15 @@
 [0:02:26] you&amp;#39;d like to explore</t>
   </si>
   <si>
+    <t>https://www.youtube.com/watch?v=hsQoHeEOZ5U</t>
+  </si>
+  <si>
+    <t>Dance with Moxie!</t>
+  </si>
+  <si>
+    <t>hsQoHeEOZ5U</t>
+  </si>
+  <si>
     <t>[0:00:00] hey Moxy let&amp;#39;s
 [0:00:03] dance oh do you want to dance with me
 [0:00:07] yes I&amp;#39;d love to dance with
@@ -2047,6 +1993,15 @@
 [0:00:54] I like dancing with
 [0:00:56] you thanks MOX that was fun L clear
 [0:01:00] ch</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=aAC6OiCil8c</t>
+  </si>
+  <si>
+    <t>Moxie's Got Jokes!</t>
+  </si>
+  <si>
+    <t>aAC6OiCil8c</t>
   </si>
   <si>
     <t>[0:00:01] hey Moxy can you tell me a
@@ -2099,6 +2054,15 @@
 [0:02:38] was funny a different one now</t>
   </si>
   <si>
+    <t>https://www.youtube.com/watch?v=vLKFfjQCa-I</t>
+  </si>
+  <si>
+    <t>LIVE NOW: Moxie now supports multiple kids!</t>
+  </si>
+  <si>
+    <t>vLKFfjQCa-I</t>
+  </si>
+  <si>
     <t>[0:00:03] hey I&amp;#39;m Daniel and this is Moxy and we
 [0:00:05] have an exciting announcement for you
 [0:00:07] coming this holiday season Moxy will be
@@ -2141,6 +2105,15 @@
 [0:01:22] us at support. body.com we can&amp;#39;t wait
 [0:01:25] for MOX to meet even more of your
 [0:01:28] family</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=bW6mZT5BL_A</t>
+  </si>
+  <si>
+    <t>One Moxie, Up to 4 Kids Profiles!</t>
+  </si>
+  <si>
+    <t>bW6mZT5BL_A</t>
   </si>
   <si>
     <t>[0:00:03] hey I&amp;#39;m Daniel and this is Moxy and we
@@ -2186,6 +2159,15 @@
 [0:01:25] for MOX to meet even more of your
 [0:01:28] family
 [0:01:33] [Music]</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=PCB0GfegoQE</t>
+  </si>
+  <si>
+    <t>Moxie's Latest Update (October 2023)</t>
+  </si>
+  <si>
+    <t>PCB0GfegoQE</t>
   </si>
   <si>
     <t>[0:00:00] hey I&amp;#39;m Daniel and more importantly this
@@ -2232,6 +2214,15 @@
 [0:01:20] Wi-Fi to download the update if you need
 [0:01:22] need help just let us
 [0:01:24] know</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=92U1BM-nLbA</t>
+  </si>
+  <si>
+    <t>Moxie Setup Demo</t>
+  </si>
+  <si>
+    <t>92U1BM-nLbA</t>
   </si>
   <si>
     <t>[0:00:00] hi everyone once again my name is Matt
@@ -2960,6 +2951,15 @@
 [0:30:23] take Moxie out</t>
   </si>
   <si>
+    <t>https://www.youtube.com/watch?v=VKJzzuuvatk</t>
+  </si>
+  <si>
+    <t>Moxie, what do you do?</t>
+  </si>
+  <si>
+    <t>VKJzzuuvatk</t>
+  </si>
+  <si>
     <t>[0:00:00] hey moxie what is it that you do
 [0:00:06] I am a curious robot named Moxie
 [0:00:08] speaking to you a young human I am an AI
@@ -2992,8 +2992,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3004,15 +3005,20 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -3025,7 +3031,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -3035,40 +3041,64 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
+  </cellStyleXfs>
+  <cellXfs count="8">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="1">
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3077,10 +3107,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -3118,69 +3148,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3204,54 +3236,53 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -3261,7 +3292,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -3270,7 +3301,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -3279,7 +3310,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -3287,10 +3318,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -3319,7 +3350,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -3332,13 +3363,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
+                <a:tint val="80000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -3356,555 +3386,534 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="1431.75">
+      <c r="A3" s="3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="520.5">
+      <c r="A4" s="3">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="428.25">
+      <c r="A5" s="3">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="454.5">
+      <c r="A6" s="3">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="876.75">
+      <c r="A7" s="3">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="1404.75">
+      <c r="A8" s="3">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="1484.25">
+      <c r="A9" s="3">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="230.25">
+      <c r="A10" s="3">
+        <v>10</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="876.75">
+      <c r="A11" s="3">
+        <v>11</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="1392">
+      <c r="A12" s="3">
+        <v>12</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="2474.25">
+      <c r="A13" s="3">
+        <v>13</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="1748.25">
+      <c r="A14" s="3">
+        <v>14</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="1893.75">
+      <c r="A15" s="3">
+        <v>15</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="1299.75">
+      <c r="A16" s="3">
+        <v>16</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E16" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="560.25">
+      <c r="A17" s="3">
+        <v>17</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="1154.25">
+      <c r="A18" s="3">
+        <v>18</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="A19" s="3">
+        <v>19</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+      <c r="A20" s="3">
+        <v>20</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+      <c r="A21" s="3">
+        <v>21</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+      <c r="A22" s="3">
+        <v>22</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+      <c r="A23" s="3">
+        <v>23</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" t="s">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+      <c r="A24" s="3">
+        <v>24</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>93</v>
       </c>
+      <c r="C24" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>96</v>
+      </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" t="s">
-        <v>94</v>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+      <c r="A25" s="3">
+        <v>25</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" t="s">
-        <v>95</v>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+      <c r="A26" s="3">
+        <v>26</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" t="s">
-        <v>96</v>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+      <c r="A27" s="3">
+        <v>27</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8" t="s">
-        <v>97</v>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+      <c r="A28" s="3">
+        <v>28</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" t="s">
-        <v>98</v>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+      <c r="A29" s="3">
+        <v>29</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" t="s">
-        <v>73</v>
-      </c>
-      <c r="E13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" t="s">
-        <v>74</v>
-      </c>
-      <c r="E14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" t="s">
-        <v>75</v>
-      </c>
-      <c r="E15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" t="s">
-        <v>79</v>
-      </c>
-      <c r="E19" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E21" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" t="s">
-        <v>82</v>
-      </c>
-      <c r="E22" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" t="s">
-        <v>83</v>
-      </c>
-      <c r="E23" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" t="s">
-        <v>84</v>
-      </c>
-      <c r="E24" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" t="s">
-        <v>85</v>
-      </c>
-      <c r="E25" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" t="s">
-        <v>86</v>
-      </c>
-      <c r="E26" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" t="s">
-        <v>87</v>
-      </c>
-      <c r="E27" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+      <c r="A30" s="3">
         <v>30</v>
       </c>
-      <c r="C28" t="s">
-        <v>59</v>
-      </c>
-      <c r="D28" t="s">
-        <v>88</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="B30" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" t="s">
-        <v>89</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="C30" s="5" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" t="s">
-        <v>90</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="D30" s="5" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" t="s">
-        <v>62</v>
-      </c>
-      <c r="D31" t="s">
-        <v>91</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="E30" s="5" t="s">
         <v>120</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="B6" r:id="rId4"/>
-    <hyperlink ref="B7" r:id="rId5"/>
-    <hyperlink ref="B8" r:id="rId6"/>
-    <hyperlink ref="B9" r:id="rId7"/>
-    <hyperlink ref="B10" r:id="rId8"/>
-    <hyperlink ref="B11" r:id="rId9"/>
-    <hyperlink ref="B12" r:id="rId10"/>
-    <hyperlink ref="B13" r:id="rId11"/>
-    <hyperlink ref="B14" r:id="rId12"/>
-    <hyperlink ref="B15" r:id="rId13"/>
-    <hyperlink ref="B16" r:id="rId14"/>
-    <hyperlink ref="B17" r:id="rId15"/>
-    <hyperlink ref="B18" r:id="rId16"/>
-    <hyperlink ref="B19" r:id="rId17"/>
-    <hyperlink ref="B20" r:id="rId18"/>
-    <hyperlink ref="B21" r:id="rId19"/>
-    <hyperlink ref="B22" r:id="rId20"/>
-    <hyperlink ref="B23" r:id="rId21"/>
-    <hyperlink ref="B24" r:id="rId22"/>
-    <hyperlink ref="B25" r:id="rId23"/>
-    <hyperlink ref="B26" r:id="rId24"/>
-    <hyperlink ref="B27" r:id="rId25"/>
-    <hyperlink ref="B28" r:id="rId26"/>
-    <hyperlink ref="B29" r:id="rId27"/>
-    <hyperlink ref="B30" r:id="rId28"/>
-    <hyperlink ref="B31" r:id="rId29"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>